<commit_message>
[fix] fill text, member count, select index
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="46">
   <si>
     <t xml:space="preserve">id_name</t>
   </si>
@@ -165,7 +165,7 @@
     <t xml:space="preserve">A210466111</t>
   </si>
   <si>
-    <t xml:space="preserve">Tom Huang</t>
+    <t xml:space="preserve">Jimmy Huang</t>
   </si>
   <si>
     <t xml:space="preserve">0918-523-190</t>
@@ -175,6 +175,43 @@
   </si>
   <si>
     <t xml:space="preserve">男</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucy Cheng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A247610447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terry Huang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A154412780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alix Wang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A178912410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linda Cheng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A215479289</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenny Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A120991307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rose Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A262456145</t>
   </si>
 </sst>
 </file>
@@ -184,7 +221,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -225,6 +262,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -268,7 +310,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,6 +331,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -306,15 +356,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,7 +417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>16</v>
       </c>
@@ -402,10 +452,10 @@
         <v>26</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>1986</v>
+        <v>1951</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>28</v>
@@ -417,7 +467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>28</v>
       </c>
@@ -452,10 +502,10 @@
         <v>26</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>1986</v>
+        <v>1961</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>28</v>
@@ -467,7 +517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>30</v>
       </c>
@@ -502,10 +552,10 @@
         <v>33</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>1986</v>
+        <v>1971</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>28</v>
@@ -514,6 +564,306 @@
         <v>27</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>1981</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>1991</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>2001</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>1950</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>1973</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -522,6 +872,12 @@
     <hyperlink ref="H2" r:id="rId1" display="sloss_huang@gmail.com"/>
     <hyperlink ref="H3" r:id="rId2" display="sloss_huang@gmail.com"/>
     <hyperlink ref="H4" r:id="rId3" display="sloss_huang@gmail.com"/>
+    <hyperlink ref="H5" r:id="rId4" display="sloss_huang@gmail.com"/>
+    <hyperlink ref="H6" r:id="rId5" display="sloss_huang@gmail.com"/>
+    <hyperlink ref="H7" r:id="rId6" display="sloss_huang@gmail.com"/>
+    <hyperlink ref="H8" r:id="rId7" display="sloss_huang@gmail.com"/>
+    <hyperlink ref="H9" r:id="rId8" display="sloss_huang@gmail.com"/>
+    <hyperlink ref="H10" r:id="rId9" display="sloss_huang@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
[fix] treate tel number as string
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="433">
   <si>
     <t xml:space="preserve">id_name</t>
   </si>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">Sloss Huang</t>
   </si>
   <si>
-    <t xml:space="preserve">0918-523-189</t>
+    <t xml:space="preserve">0918523189</t>
   </si>
   <si>
     <t xml:space="preserve">台北市</t>
@@ -139,9 +139,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">0918-523-188</t>
-  </si>
-  <si>
     <t xml:space="preserve">na</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cacy Huang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0918523190</t>
   </si>
   <si>
     <t xml:space="preserve">新北市</t>
@@ -231,7 +231,7 @@
     <t xml:space="preserve">Jimmy Huang</t>
   </si>
   <si>
-    <t xml:space="preserve">0918-523-190</t>
+    <t xml:space="preserve">0918523191</t>
   </si>
   <si>
     <t xml:space="preserve">其他(other)</t>
@@ -246,6 +246,9 @@
     <t xml:space="preserve">Lucy Cheng</t>
   </si>
   <si>
+    <t xml:space="preserve">0918523192</t>
+  </si>
+  <si>
     <t xml:space="preserve">高雄市</t>
   </si>
   <si>
@@ -258,6 +261,9 @@
     <t xml:space="preserve">Terry Huang</t>
   </si>
   <si>
+    <t xml:space="preserve">0918523193</t>
+  </si>
+  <si>
     <t xml:space="preserve">宜蘭縣</t>
   </si>
   <si>
@@ -268,6 +274,9 @@
   </si>
   <si>
     <t xml:space="preserve">Alix Wang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0918523194</t>
   </si>
   <si>
     <t xml:space="preserve">桃園市</t>
@@ -283,6 +292,9 @@
     <t xml:space="preserve">Linda Cheng</t>
   </si>
   <si>
+    <t xml:space="preserve">0918523195</t>
+  </si>
+  <si>
     <t xml:space="preserve">嘉義市</t>
   </si>
   <si>
@@ -295,6 +307,9 @@
     <t xml:space="preserve">Kenny Lee</t>
   </si>
   <si>
+    <t xml:space="preserve">0918523196</t>
+  </si>
+  <si>
     <t xml:space="preserve">新竹縣</t>
   </si>
   <si>
@@ -305,6 +320,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rose Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0918523197</t>
   </si>
   <si>
     <t xml:space="preserve">彰化縣</t>
@@ -1431,8 +1449,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1549,7 +1568,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1563,6 +1582,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1613,8 +1636,8 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1689,7 +1712,7 @@
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1698,26 +1721,26 @@
       <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="L2" s="3" t="n">
         <v>1951</v>
@@ -1729,18 +1752,18 @@
         <v>28</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>29</v>
@@ -1748,26 +1771,26 @@
       <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="3" t="n">
         <v>1961</v>
@@ -1779,17 +1802,17 @@
         <v>28</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1798,20 +1821,20 @@
       <c r="D4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>36</v>
@@ -1829,45 +1852,45 @@
         <v>28</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
+      <c r="B5" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="J5" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5" s="3" t="n">
         <v>1981</v>
@@ -1879,42 +1902,42 @@
         <v>28</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="J6" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>37</v>
@@ -1929,42 +1952,42 @@
         <v>28</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>48</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>49</v>
+      <c r="J7" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>37</v>
@@ -1979,45 +2002,45 @@
         <v>28</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>53</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="J8" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8" s="3" t="n">
         <v>2011</v>
@@ -2029,42 +2052,42 @@
         <v>28</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>58</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="J9" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>37</v>
@@ -2079,45 +2102,45 @@
         <v>28</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="J10" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10" s="3" t="n">
         <v>1973</v>
@@ -2129,10 +2152,10 @@
         <v>28</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2402,1267 +2425,1267 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
+      <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>74</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>75</v>
+      <c r="A3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>64</v>
+      <c r="A4" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="10" t="s">
+      <c r="B5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="G5" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="H5" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="I5" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="J5" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="K5" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="L5" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="M5" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="N5" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="U5" s="10" t="s">
+      <c r="O5" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="V5" s="10" t="s">
+      <c r="P5" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="W5" s="10" t="s">
+      <c r="Q5" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="R5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="S5" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="Z5" s="10" t="s">
+      <c r="T5" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="AA5" s="10" t="s">
+      <c r="U5" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="AB5" s="10" t="s">
+      <c r="V5" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="AC5" s="10" t="s">
+      <c r="W5" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="AD5" s="10" t="s">
+      <c r="X5" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="AE5" s="10" t="s">
+      <c r="Y5" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="AF5" s="10" t="s">
+      <c r="Z5" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="AG5" s="10" t="s">
+      <c r="AA5" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="AH5" s="10" t="s">
+      <c r="AB5" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="AI5" s="10" t="s">
+      <c r="AC5" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AJ5" s="10" t="s">
+      <c r="AD5" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="AK5" s="10" t="s">
+      <c r="AE5" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AL5" s="10" t="s">
+      <c r="AF5" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AM5" s="10" t="s">
+      <c r="AG5" s="11" t="s">
         <v>117</v>
+      </c>
+      <c r="AH5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI5" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK5" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM5" s="11" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="G6" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="H6" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="I6" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="J6" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="K6" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="L6" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="M6" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="N6" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="U6" s="10" t="s">
+      <c r="O6" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="V6" s="10" t="s">
+      <c r="P6" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="W6" s="10" t="s">
+      <c r="Q6" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="X6" s="10" t="s">
+      <c r="R6" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="Y6" s="10" t="s">
+      <c r="S6" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="Z6" s="10" t="s">
+      <c r="T6" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AA6" s="10" t="s">
+      <c r="U6" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="AB6" s="10" t="s">
+      <c r="V6" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="AC6" s="10" t="s">
+      <c r="W6" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="AD6" s="10" t="s">
+      <c r="X6" s="11" t="s">
         <v>145</v>
+      </c>
+      <c r="Y6" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z6" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA6" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB6" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD6" s="11" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="I7" s="10" t="s">
+      <c r="A7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="G7" s="11" t="s">
         <v>156</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="I8" s="10" t="s">
+      <c r="A8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="G8" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="H8" s="11" t="s">
         <v>168</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>169</v>
+      <c r="A9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="H10" s="10" t="s">
+      <c r="A10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="E10" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="F10" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="G10" s="11" t="s">
         <v>181</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="C11" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="E11" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="G11" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="H11" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="I11" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="J11" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="Q11" s="10" t="s">
+      <c r="K11" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="R11" s="10" t="s">
+      <c r="L11" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="S11" s="10" t="s">
+      <c r="M11" s="11" t="s">
         <v>200</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="S11" s="11" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="C12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="E12" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="G12" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="H12" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="I12" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="J12" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="Q12" s="10" t="s">
+      <c r="K12" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="R12" s="10" t="s">
+      <c r="L12" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="S12" s="10" t="s">
+      <c r="M12" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="T12" s="10" t="s">
+      <c r="N12" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="U12" s="10" t="s">
+      <c r="O12" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="V12" s="10" t="s">
+      <c r="P12" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="W12" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="X12" s="10" t="s">
+      <c r="Q12" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="Y12" s="10" t="s">
+      <c r="R12" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="Z12" s="10" t="s">
+      <c r="S12" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="AA12" s="10" t="s">
+      <c r="T12" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="AB12" s="10" t="s">
+      <c r="U12" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="AC12" s="10" t="s">
+      <c r="V12" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="AD12" s="10" t="s">
+      <c r="W12" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="X12" s="11" t="s">
         <v>227</v>
+      </c>
+      <c r="Y12" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z12" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA12" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB12" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC12" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="AD12" s="11" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="G13" s="10" t="s">
+      <c r="A13" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="D13" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="E13" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="F13" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="G13" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="H13" s="11" t="s">
         <v>241</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="I14" s="10" t="s">
+      <c r="A14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="E14" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="F14" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="G14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="O14" s="10" t="s">
+      <c r="I14" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="J14" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="Q14" s="10" t="s">
+      <c r="K14" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="R14" s="10" t="s">
+      <c r="L14" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="S14" s="10" t="s">
+      <c r="M14" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="T14" s="10" t="s">
+      <c r="N14" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="U14" s="10" t="s">
+      <c r="O14" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="V14" s="10" t="s">
+      <c r="P14" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="W14" s="10" t="s">
+      <c r="Q14" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="X14" s="10" t="s">
+      <c r="R14" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="Y14" s="10" t="s">
+      <c r="S14" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="Z14" s="10" t="s">
+      <c r="T14" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="AA14" s="10" t="s">
+      <c r="U14" s="11" t="s">
         <v>266</v>
+      </c>
+      <c r="V14" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="W14" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="X14" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="Y14" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="Z14" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="AA14" s="11" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>268</v>
+      <c r="A15" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="G16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="E16" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="M16" s="10" t="s">
+      <c r="G16" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="N16" s="10" t="s">
+      <c r="H16" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="O16" s="10" t="s">
+      <c r="I16" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="J16" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="Q16" s="10" t="s">
+      <c r="K16" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="R16" s="10" t="s">
+      <c r="L16" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="S16" s="10" t="s">
+      <c r="M16" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="T16" s="10" t="s">
+      <c r="N16" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="U16" s="10" t="s">
+      <c r="O16" s="11" t="s">
         <v>289</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q16" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="T16" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="G17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="B17" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="D17" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="E17" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="F17" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="G17" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="N17" s="10" t="s">
+      <c r="H17" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="I17" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="P17" s="10" t="s">
+      <c r="J17" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="Q17" s="10" t="s">
+      <c r="K17" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="R17" s="10" t="s">
+      <c r="L17" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="S17" s="10" t="s">
+      <c r="M17" s="11" t="s">
         <v>308</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="G18" s="10" t="s">
+      <c r="A18" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="B18" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="C18" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="D18" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="E18" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="F18" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="G18" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="H18" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="O18" s="10" t="s">
+      <c r="I18" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="P18" s="10" t="s">
+      <c r="J18" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="Q18" s="10" t="s">
+      <c r="K18" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="R18" s="10" t="s">
+      <c r="L18" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="S18" s="10" t="s">
+      <c r="M18" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="T18" s="10" t="s">
+      <c r="N18" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="U18" s="10" t="s">
+      <c r="O18" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="V18" s="10" t="s">
+      <c r="P18" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="W18" s="10" t="s">
+      <c r="Q18" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="X18" s="10" t="s">
+      <c r="R18" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="Y18" s="10" t="s">
+      <c r="S18" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="Z18" s="10" t="s">
+      <c r="T18" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="AA18" s="10" t="s">
+      <c r="U18" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="AB18" s="10" t="s">
+      <c r="V18" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="AC18" s="10" t="s">
+      <c r="W18" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="AD18" s="10" t="s">
+      <c r="X18" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="AE18" s="10" t="s">
+      <c r="Y18" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="AF18" s="10" t="s">
+      <c r="Z18" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="AG18" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH18" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="AI18" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="AJ18" s="10" t="s">
+      <c r="AA18" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="AK18" s="10" t="s">
+      <c r="AB18" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="AL18" s="10" t="s">
+      <c r="AC18" s="11" t="s">
         <v>343</v>
+      </c>
+      <c r="AD18" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="AE18" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="AF18" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="AG18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH18" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI18" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="AJ18" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="AK18" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="AL18" s="11" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>345</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="G19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="C19" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="D19" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="E19" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="F19" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="M19" s="10" t="s">
+      <c r="G19" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="H19" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="O19" s="10" t="s">
+      <c r="I19" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="J19" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="Q19" s="10" t="s">
+      <c r="K19" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="R19" s="10" t="s">
+      <c r="L19" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="S19" s="10" t="s">
+      <c r="M19" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="T19" s="10" t="s">
+      <c r="N19" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="U19" s="10" t="s">
+      <c r="O19" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="V19" s="10" t="s">
+      <c r="P19" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="W19" s="10" t="s">
+      <c r="Q19" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="X19" s="10" t="s">
+      <c r="R19" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="Y19" s="10" t="s">
+      <c r="S19" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="Z19" s="10" t="s">
+      <c r="T19" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="AA19" s="10" t="s">
+      <c r="U19" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="AB19" s="10" t="s">
+      <c r="V19" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="AC19" s="10" t="s">
+      <c r="W19" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="AD19" s="10" t="s">
+      <c r="X19" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="AE19" s="10" t="s">
+      <c r="Y19" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="AF19" s="10" t="s">
+      <c r="Z19" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="AG19" s="10" t="s">
+      <c r="AA19" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="AH19" s="10" t="s">
+      <c r="AB19" s="11" t="s">
         <v>377</v>
+      </c>
+      <c r="AC19" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="AD19" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="AE19" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="AF19" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="AG19" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="AH19" s="11" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="G20" s="10" t="s">
+      <c r="A20" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="B20" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="D20" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="E20" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="F20" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="G20" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="N20" s="10" t="s">
+      <c r="H20" s="11" t="s">
         <v>391</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="B21" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="C21" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="D21" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="K21" s="10" t="s">
+      <c r="E21" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="F21" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="G21" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="N21" s="10" t="s">
+      <c r="H21" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="O21" s="10" t="s">
+      <c r="I21" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="P21" s="10" t="s">
+      <c r="J21" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="Q21" s="10" t="s">
+      <c r="K21" s="11" t="s">
         <v>408</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="O21" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q21" s="11" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>414</v>
+      <c r="A22" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>417</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="G23" s="10" t="s">
+      <c r="A23" s="11" t="s">
         <v>421</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>426</v>
+      <c r="A24" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[add] stay auto fill
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="member" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="cnt" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="stay" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="436">
   <si>
     <t xml:space="preserve">id_name</t>
   </si>
@@ -378,6 +379,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">其他</t>
     </r>
@@ -1443,6 +1445,15 @@
   </si>
   <si>
     <t xml:space="preserve">東引鄉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomas Huang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0918523288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tomas_huang@google.com</t>
   </si>
 </sst>
 </file>
@@ -1516,8 +1527,10 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Noto Sans CJK SC Regular"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1568,7 +1581,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1609,8 +1622,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1636,26 +1653,26 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49489795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.4234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.6428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,7 +2360,7 @@
   </sheetData>
   <dataValidations count="11">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2 I2" type="list">
-      <formula1>"中華民國,"</formula1>
+      <formula1>"中華民國"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="equal" prompt="請選擇縣市" promptTitle="請選擇縣市" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C10" type="list">
@@ -2421,7 +2438,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3706,4 +3723,59 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>435</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="tomas_huang@google.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[add] readme on sample.xlsx
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="member" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="cnt" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="readme" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="member" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="stay" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="cnt" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="442">
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tab </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">名稱</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">說明</t>
+  </si>
+  <si>
+    <t xml:space="preserve">member</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">領隊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">第一位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">隊員詳細資料</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">stay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">留守人員詳細資料</t>
+  </si>
   <si>
     <t xml:space="preserve">id_name</t>
   </si>
@@ -335,6 +413,15 @@
     <t xml:space="preserve">A262456145</t>
   </si>
   <si>
+    <t xml:space="preserve">Tomas Huang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0918523288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tomas_huang@google.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Country</t>
   </si>
   <si>
@@ -1446,15 +1533,6 @@
   <si>
     <t xml:space="preserve">東引鄉</t>
   </si>
-  <si>
-    <t xml:space="preserve">Tomas Huang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0918523288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tomas_huang@google.com</t>
-  </si>
 </sst>
 </file>
 
@@ -1464,7 +1542,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1488,10 +1566,27 @@
     </font>
     <font>
       <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1520,14 +1615,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1581,32 +1676,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1614,20 +1721,20 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1651,528 +1758,581 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="43.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    <row r="1" s="5" customFormat="true" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="E2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="6" t="n">
         <v>1951</v>
       </c>
-      <c r="M2" s="3" t="n">
+      <c r="M2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="3" t="n">
+      <c r="N2" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>17</v>
+      <c r="O2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="H3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="I3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="J3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="L3" s="6" t="n">
+        <v>1961</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="O3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>1961</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>28</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>28</v>
+      <c r="P3" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="A4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="F4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="6" t="n">
         <v>1971</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="N4" s="3" t="n">
+      <c r="N4" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>34</v>
+      <c r="O4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="A5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="6" t="n">
         <v>1981</v>
       </c>
-      <c r="M5" s="3" t="n">
+      <c r="M5" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="N5" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>39</v>
+      <c r="O5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="6" t="n">
         <v>1991</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="N6" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>44</v>
+      <c r="O6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="A7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="F7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="6" t="n">
         <v>2001</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="M7" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="N7" s="3" t="n">
+      <c r="N7" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>49</v>
+      <c r="O7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="A8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="3" t="n">
+      <c r="L8" s="6" t="n">
         <v>2011</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="M8" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="N8" s="3" t="n">
+      <c r="N8" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>54</v>
+      <c r="O8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="A9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="F9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="6" t="n">
         <v>1950</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="M9" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="N9" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>59</v>
+      <c r="O9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="A10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="6" t="n">
         <v>1973</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="M10" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="N10" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>64</v>
+      <c r="O10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2425,7 +2585,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="tomas_huang@google.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2437,1272 +2652,1269 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
+      <c r="A1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="11" t="s">
+      <c r="A2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="D2" s="15" t="s">
         <v>80</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>81</v>
+      <c r="A3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>70</v>
+      <c r="C4" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="L5" s="11" t="s">
+      <c r="A5" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="D5" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="E5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="F5" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="G5" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="H5" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="I5" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="J5" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="K5" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="L5" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="V5" s="11" t="s">
+      <c r="M5" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="W5" s="11" t="s">
+      <c r="N5" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="X5" s="11" t="s">
+      <c r="O5" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="P5" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="Z5" s="11" t="s">
+      <c r="Q5" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="AA5" s="11" t="s">
+      <c r="R5" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="AB5" s="11" t="s">
+      <c r="S5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="AC5" s="11" t="s">
+      <c r="T5" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="AD5" s="11" t="s">
+      <c r="U5" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="AE5" s="11" t="s">
+      <c r="V5" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="AF5" s="11" t="s">
+      <c r="W5" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="AG5" s="11" t="s">
+      <c r="X5" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="AH5" s="11" t="s">
+      <c r="Y5" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="AI5" s="11" t="s">
+      <c r="Z5" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="AJ5" s="11" t="s">
+      <c r="AA5" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="AK5" s="11" t="s">
+      <c r="AB5" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="AL5" s="11" t="s">
+      <c r="AC5" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="AM5" s="11" t="s">
+      <c r="AD5" s="15" t="s">
         <v>123</v>
+      </c>
+      <c r="AE5" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF5" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG5" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH5" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI5" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ5" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AK5" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL5" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM5" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="L6" s="11" t="s">
+      <c r="A6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="D6" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="E6" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="F6" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="G6" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="H6" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="I6" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="J6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="K6" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="L6" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="M6" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="N6" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="O6" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Y6" s="11" t="s">
+      <c r="P6" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="Z6" s="11" t="s">
+      <c r="Q6" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="AA6" s="11" t="s">
+      <c r="R6" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="AB6" s="11" t="s">
+      <c r="S6" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="AC6" s="11" t="s">
+      <c r="T6" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="AD6" s="11" t="s">
+      <c r="U6" s="15" t="s">
         <v>151</v>
+      </c>
+      <c r="V6" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="W6" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="X6" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y6" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z6" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA6" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB6" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC6" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD6" s="15" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="L7" s="11" t="s">
+      <c r="A7" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="C7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>162</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="L8" s="11" t="s">
+      <c r="A8" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="C8" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="E8" s="15" t="s">
         <v>174</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>175</v>
+      <c r="A9" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="L10" s="11" t="s">
+      <c r="A10" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="C10" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="D10" s="15" t="s">
         <v>187</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="J11" s="11" t="s">
+      <c r="A11" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="B11" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="C11" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="D11" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="E11" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="F11" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="P11" s="11" t="s">
+      <c r="G11" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="Q11" s="11" t="s">
+      <c r="H11" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="I11" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="S11" s="11" t="s">
+      <c r="J11" s="15" t="s">
         <v>206</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="S11" s="15" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="L12" s="11" t="s">
+      <c r="A12" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="B12" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="N12" s="11" t="s">
+      <c r="C12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="E12" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="P12" s="11" t="s">
+      <c r="G12" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="Q12" s="11" t="s">
+      <c r="H12" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="R12" s="11" t="s">
+      <c r="I12" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="S12" s="11" t="s">
+      <c r="J12" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="T12" s="11" t="s">
+      <c r="K12" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="U12" s="11" t="s">
+      <c r="L12" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="V12" s="11" t="s">
+      <c r="M12" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="W12" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="X12" s="11" t="s">
+      <c r="N12" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="Y12" s="11" t="s">
+      <c r="O12" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="Z12" s="11" t="s">
+      <c r="P12" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="AA12" s="11" t="s">
+      <c r="Q12" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="AB12" s="11" t="s">
+      <c r="R12" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="AC12" s="11" t="s">
+      <c r="S12" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="AD12" s="11" t="s">
+      <c r="T12" s="15" t="s">
         <v>233</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="V12" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="W12" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="X12" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="Y12" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z12" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="AA12" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="AB12" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC12" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="AD12" s="15" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="J13" s="11" t="s">
+      <c r="A13" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="B13" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="C13" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="D13" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="N13" s="11" t="s">
+      <c r="E13" s="15" t="s">
         <v>247</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="L14" s="11" t="s">
+      <c r="A14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="C14" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="N14" s="11" t="s">
+      <c r="D14" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="O14" s="11" t="s">
+      <c r="E14" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="F14" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="Q14" s="11" t="s">
+      <c r="G14" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="I14" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="S14" s="11" t="s">
+      <c r="J14" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="T14" s="11" t="s">
+      <c r="K14" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="U14" s="11" t="s">
+      <c r="L14" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="V14" s="11" t="s">
+      <c r="M14" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="W14" s="11" t="s">
+      <c r="N14" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="X14" s="11" t="s">
+      <c r="O14" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="Y14" s="11" t="s">
+      <c r="P14" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="Z14" s="11" t="s">
+      <c r="Q14" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="AA14" s="11" t="s">
+      <c r="R14" s="15" t="s">
         <v>272</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="T14" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="U14" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="V14" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="W14" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="X14" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y14" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z14" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA14" s="15" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>274</v>
+      <c r="A15" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>278</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="J16" s="11" t="s">
+      <c r="A16" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="B16" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="C16" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="D16" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="E16" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="O16" s="11" t="s">
+      <c r="F16" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="G16" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="H16" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="I16" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="J16" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="T16" s="11" t="s">
+      <c r="K16" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="U16" s="11" t="s">
+      <c r="L16" s="15" t="s">
         <v>295</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q16" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="T16" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="U16" s="15" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="J17" s="11" t="s">
+      <c r="A17" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="B17" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="C17" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="D17" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="E17" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="O17" s="11" t="s">
+      <c r="F17" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="P17" s="11" t="s">
+      <c r="G17" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="H17" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="R17" s="11" t="s">
+      <c r="I17" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="S17" s="11" t="s">
+      <c r="J17" s="15" t="s">
         <v>314</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q17" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>322</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="J18" s="11" t="s">
+      <c r="A18" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="B18" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="C18" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="D18" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="E18" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="O18" s="11" t="s">
+      <c r="F18" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="P18" s="11" t="s">
+      <c r="G18" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="Q18" s="11" t="s">
+      <c r="H18" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="R18" s="11" t="s">
+      <c r="I18" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="S18" s="11" t="s">
+      <c r="J18" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="T18" s="11" t="s">
+      <c r="K18" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="U18" s="11" t="s">
+      <c r="L18" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="V18" s="11" t="s">
+      <c r="M18" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="W18" s="11" t="s">
+      <c r="N18" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="X18" s="11" t="s">
+      <c r="O18" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="Y18" s="11" t="s">
+      <c r="P18" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="Z18" s="11" t="s">
+      <c r="Q18" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="AA18" s="11" t="s">
+      <c r="R18" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="AB18" s="11" t="s">
+      <c r="S18" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="AC18" s="11" t="s">
+      <c r="T18" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="AD18" s="11" t="s">
+      <c r="U18" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="AE18" s="11" t="s">
+      <c r="V18" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="AF18" s="11" t="s">
+      <c r="W18" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="AG18" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH18" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="AI18" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="AJ18" s="11" t="s">
+      <c r="X18" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="AK18" s="11" t="s">
+      <c r="Y18" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="AL18" s="11" t="s">
+      <c r="Z18" s="15" t="s">
         <v>349</v>
+      </c>
+      <c r="AA18" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="AB18" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="AC18" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="AD18" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE18" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="AF18" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="AG18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH18" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="AI18" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AJ18" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="AK18" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="AL18" s="15" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="J19" s="11" t="s">
+      <c r="A19" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="B19" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="C19" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="D19" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="E19" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="O19" s="11" t="s">
+      <c r="F19" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="P19" s="11" t="s">
+      <c r="G19" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="Q19" s="11" t="s">
+      <c r="H19" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="R19" s="11" t="s">
+      <c r="I19" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="S19" s="11" t="s">
+      <c r="J19" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="T19" s="11" t="s">
+      <c r="K19" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="U19" s="11" t="s">
+      <c r="L19" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="V19" s="11" t="s">
+      <c r="M19" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="W19" s="11" t="s">
+      <c r="N19" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="X19" s="11" t="s">
+      <c r="O19" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="Y19" s="11" t="s">
+      <c r="P19" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="Z19" s="11" t="s">
+      <c r="Q19" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="AA19" s="11" t="s">
+      <c r="R19" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="AB19" s="11" t="s">
+      <c r="S19" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="AC19" s="11" t="s">
+      <c r="T19" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="AD19" s="11" t="s">
+      <c r="U19" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="AE19" s="11" t="s">
+      <c r="V19" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="AF19" s="11" t="s">
+      <c r="W19" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="AG19" s="11" t="s">
+      <c r="X19" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="AH19" s="11" t="s">
+      <c r="Y19" s="15" t="s">
         <v>383</v>
+      </c>
+      <c r="Z19" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="AA19" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="AB19" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="AC19" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="AD19" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="AE19" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="AF19" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="AG19" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="AH19" s="15" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
-        <v>384</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>385</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>389</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>391</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="J20" s="11" t="s">
+      <c r="A20" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="B20" s="15" t="s">
         <v>394</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="C20" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="D20" s="15" t="s">
         <v>396</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="E20" s="15" t="s">
         <v>397</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
-        <v>398</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="J21" s="11" t="s">
+      <c r="A21" s="15" t="s">
         <v>407</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="B21" s="15" t="s">
         <v>408</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="C21" s="15" t="s">
         <v>409</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="D21" s="15" t="s">
         <v>410</v>
       </c>
-      <c r="N21" s="11" t="s">
+      <c r="E21" s="15" t="s">
         <v>411</v>
       </c>
-      <c r="O21" s="11" t="s">
+      <c r="F21" s="15" t="s">
         <v>412</v>
       </c>
-      <c r="P21" s="11" t="s">
+      <c r="G21" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="Q21" s="11" t="s">
+      <c r="H21" s="15" t="s">
         <v>414</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q21" s="15" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>420</v>
+      <c r="A22" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>427</v>
+      <c r="A23" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>429</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>431</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>432</v>
+      <c r="A24" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -3723,59 +3935,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>435</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="tomas_huang@google.com"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>